<commit_message>
updated rollout wil template
</commit_message>
<xml_diff>
--- a/templates/IssueBluePrintRolloutWIL.xlsx
+++ b/templates/IssueBluePrintRolloutWIL.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27823"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hypatos.sharepoint.com/sites/Projects/Freigegebene Dokumente/Wilhelmsen/02 PM/Rollout Jira Blueprint/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephankuche/CreateJiraIssues/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E427A3B-D65A-4617-AF27-E61DBE2E0613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EB71B3-1233-9F43-8E93-C1A778BE6E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4500" yWindow="1460" windowWidth="35840" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WilhIssueBluePrintRollout" sheetId="16" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="17" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">WilhIssueBluePrintRollout!$A$1:$G$114</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="134">
   <si>
     <t>Summary</t>
   </si>
@@ -62,92 +63,41 @@
     <t>Duration</t>
   </si>
   <si>
-    <t>Roll-out Wilhelmsen</t>
-  </si>
-  <si>
     <t>Project</t>
   </si>
   <si>
-    <t>0. Project Management</t>
-  </si>
-  <si>
     <t>Epic</t>
   </si>
   <si>
-    <t>0_1 - Update_all_related_dates_in_this_project</t>
-  </si>
-  <si>
     <t>Task</t>
   </si>
   <si>
-    <t>0_2 - Update_roll-out_plan</t>
-  </si>
-  <si>
     <t>File : https://wilhelmsen.sharepoint.com/:f:/r/sites/Wilhelmsen-HypatosDigitalization/Shared%20Documents/PMO/Rollout%20Plan?csf=1&amp;web=1&amp;e=eIf44E</t>
   </si>
   <si>
-    <t>0_3 - Internal_meetings</t>
-  </si>
-  <si>
     <t xml:space="preserve">Task to log general internal meetings </t>
   </si>
   <si>
-    <t>1. Process Discovery</t>
-  </si>
-  <si>
-    <t>1_1 - Data_Acquisition</t>
-  </si>
-  <si>
-    <t>1_2 - Requirement_Gathering</t>
-  </si>
-  <si>
-    <t>Training &amp; Posting Data Request</t>
-  </si>
-  <si>
     <t>Sub-task</t>
   </si>
   <si>
-    <t>Posting Data Analysis</t>
-  </si>
-  <si>
     <t>Analyze posting data and determine top suppliers (&gt;90% coverage)</t>
   </si>
   <si>
-    <t>Training Data Assessment</t>
-  </si>
-  <si>
     <t>Check if all top suppliers has sample documents with specified naming convention</t>
   </si>
   <si>
-    <t>Request additional documents if required</t>
-  </si>
-  <si>
     <t>Request if any top supplier document is missing</t>
   </si>
   <si>
-    <t>Training Data/Document Set Preparation</t>
-  </si>
-  <si>
     <t>Prepare training, annotation documents</t>
   </si>
   <si>
-    <t>Match training documents with posting data</t>
-  </si>
-  <si>
     <t>Match selected documents with posting data</t>
-  </si>
-  <si>
-    <t>2_1 - Capturing_Model_Training,2_2 - Enrichment_Model_Training</t>
-  </si>
-  <si>
-    <t>Provide Digitalization Details form to Local Finance Team and ask examples for Edge cases</t>
   </si>
   <si>
     <t>EXAMPLE DOCUMENT
 https://wilhelmsen.sharepoint.com/:x:/r/sites/Wilhelmsen-HypatosDigitalization/Shared%20Documents/General/2.%20-%20Workshops/Assessment%20Workshop/Digitalization%20details%20for%20Hypatos_Country.xlsx?d=w1f4142a7ac7a4094a18dd8c9455cf25d&amp;csf=1&amp;web=1&amp;e=DJWR4y</t>
-  </si>
-  <si>
-    <t>Provide Assessment Gathering  and Training  Data  Folders</t>
   </si>
   <si>
     <t xml:space="preserve">Assessment Folders : https://wilhelmsen.sharepoint.com/:f:/r/sites/Wilhelmsen-HypatosDigitalization/Shared%20Documents/General/2.%20-%20Workshops/Assessment%20Workshop
@@ -155,302 +105,353 @@
 </t>
   </si>
   <si>
-    <t>[ML] Demo Project Creation for Requirements Gathering Meeting</t>
-  </si>
-  <si>
     <t>Take the example from [ML] Project - [OC Entities][Phase 3] Oman</t>
   </si>
   <si>
-    <t>Requirement Gathering Meeting</t>
-  </si>
-  <si>
-    <t>Request examples for Edge cases</t>
-  </si>
-  <si>
-    <t>Complete full set-up of training data for all of the top suppliers with Edge cases shared during requirements session</t>
-  </si>
-  <si>
-    <t>Update WHL Requirement List</t>
-  </si>
-  <si>
     <t>https://wilhelmsen.sharepoint.com/:x:/r/sites/Wilhelmsen-HypatosDigitalization/Shared%20Documents/Solution%20Design/Datapoint_Requirements/20230803%20WHL%20Requirement%20List.xlsx?d=wa1d0a15e28594d848e8def48ff3796e2&amp;csf=1&amp;web=1&amp;e=hxnCwT</t>
   </si>
   <si>
-    <t>Requirement Gathering Finalization</t>
-  </si>
-  <si>
-    <t>2. Model Training</t>
-  </si>
-  <si>
-    <t>2_1 - Capturing_Model_Training</t>
-  </si>
-  <si>
-    <t>2_3 - Model_Fine_Tuning</t>
-  </si>
-  <si>
-    <t>Create baseline (groundtruth) project to annotate [ML]</t>
-  </si>
-  <si>
     <t>Take the example from [ML] Project - NZ_Annotation</t>
   </si>
   <si>
-    <t>Upload documents selected for annotation to groundtruth project (Top suppliers and Edge cases)</t>
-  </si>
-  <si>
-    <t>Create a task for annotation (add details per requirements)</t>
-  </si>
-  <si>
-    <t>Validate annotation results with posting data</t>
-  </si>
-  <si>
-    <t>Improve annotation quality based on validation with posting data</t>
-  </si>
-  <si>
-    <t>Create Training  Project [ML]</t>
-  </si>
-  <si>
     <t>Take the example from[ML] Project - [Training][PROD][NZ]</t>
   </si>
   <si>
-    <t>Upload selected training documents from baseline project to Training Project [ML]</t>
-  </si>
-  <si>
-    <t>Create  QA Project [ML]</t>
-  </si>
-  <si>
     <t>Take the example from [ML] Project -  [QA] NZ</t>
   </si>
   <si>
-    <t>Configure QA project with Composite Enrichment Index</t>
-  </si>
-  <si>
-    <t>Create LLM Prompting Service [ML]</t>
-  </si>
-  <si>
-    <t>Upload baseline (groundtruth) documents to QA Project [ML]</t>
-  </si>
-  <si>
-    <t>Create Error Analysis Dashboard</t>
-  </si>
-  <si>
-    <t>Analyze QA results and accuracy</t>
-  </si>
-  <si>
-    <t>2_2 - Enrichment_Model_Training</t>
-  </si>
-  <si>
-    <t>Create IMP training project [TEST]</t>
-  </si>
-  <si>
-    <t>Contact with IM to enable IMP pipeline</t>
-  </si>
-  <si>
-    <t>Upload documents to IMP training project</t>
-  </si>
-  <si>
-    <t>Train suppliers using documents uploaded to IMP project</t>
-  </si>
-  <si>
-    <t>3_1 - Create_Projects_[TEST]</t>
-  </si>
-  <si>
-    <t>Improve/Optimize  LLM Prompting Service prompt with Error Analysis results</t>
-  </si>
-  <si>
-    <t>Add additional suppliers to IMP project if required</t>
-  </si>
-  <si>
-    <t>3.Studio Configuration</t>
-  </si>
-  <si>
-    <t>3_2 - Configure_Projects_[TEST]</t>
-  </si>
-  <si>
-    <t>Configure project schema with agreed upon requirements lists points</t>
-  </si>
-  <si>
-    <t>Add/Change accounting supplier/customer  party</t>
-  </si>
-  <si>
-    <t>Add/Change  company name validation</t>
-  </si>
-  <si>
-    <t>Add/check vat id validation</t>
-  </si>
-  <si>
-    <t>Check/change duplicate source data point</t>
-  </si>
-  <si>
-    <t>(Optional) Add translation data points if required</t>
-  </si>
-  <si>
-    <t>4_1 - Testing_Set-up</t>
-  </si>
-  <si>
-    <t>Create a COE ticket to configure Rerouting rules</t>
-  </si>
-  <si>
     <t>Example task : https://hypatos.atlassian.net/browse/WHL-825</t>
   </si>
   <si>
-    <t>Contact IM for composite enrichment set-up configuration</t>
-  </si>
-  <si>
-    <t>Contact IM to create and configure LLM prompting service</t>
-  </si>
-  <si>
-    <t>Contact IM to enable newly created [TEST] outbound projects for duplicate check pipeline (Connect projects to IMP pipeline)</t>
-  </si>
-  <si>
-    <t>Contact IM to add outbound projects to XML UBL 2.1 endpoint [TEST]</t>
-  </si>
-  <si>
-    <t>Contact IM to enable translation for outbound projects</t>
-  </si>
-  <si>
-    <t>4.  Testing</t>
-  </si>
-  <si>
-    <t>4_2 - Functional_Testing_by_HY</t>
-  </si>
-  <si>
-    <t>Copy and update Test Workbook for new phase if needed</t>
-  </si>
-  <si>
     <t>Example Workbook: https://wilhelmsen.sharepoint.com/:x:/r/sites/Wilhelmsen-HypatosDigitalization/Shared%20Documents/Testing/20240219_WILH_TestWorkbook.xlsx?d=w69cb18348f0b4ca7b8673d2b6069bc2d&amp;csf=1&amp;web=1&amp;e=XKhJvy</t>
   </si>
   <si>
-    <t>4_3 - Testing_by_Wilhelmsen</t>
-  </si>
-  <si>
-    <t>Compare project set-up with requirements list for specific country</t>
-  </si>
-  <si>
     <t>Requirements Sheet: https://wilhelmsen.sharepoint.com/:x:/r/sites/Wilhelmsen-HypatosDigitalization/Shared%20Documents/Solution%20Design/Datapoint_Requirements/20230803%20WHL%20Requirement%20List.xlsx?d=wa1d0a15e28594d848e8def48ff3796e2&amp;csf=1&amp;web=1&amp;e=hxnCwT</t>
   </si>
   <si>
-    <t>Upload documents to Gateway project and test routing</t>
-  </si>
-  <si>
-    <t>Test advanced duplicate testing</t>
-  </si>
-  <si>
-    <t>Test if enrichment is working properly with company code filter</t>
-  </si>
-  <si>
-    <t>Test if XML endpoint if available for outbound projects (Postman)</t>
-  </si>
-  <si>
-    <t>[Optional] Test translation feature</t>
-  </si>
-  <si>
-    <t>5_1 - Create_Projects_[PROD]</t>
-  </si>
-  <si>
-    <t>Add projects to Requirements List</t>
-  </si>
-  <si>
-    <t>Share Test Workbook</t>
-  </si>
-  <si>
-    <t>Wilhelmsen to configure integration &amp; perform System Integration Testing (SIT)</t>
-  </si>
-  <si>
-    <t>Wilhelmsen to perform Functional Testing</t>
-  </si>
-  <si>
-    <t>Wilhelmsen to perform User Acceptance Testing (UAT)</t>
-  </si>
-  <si>
-    <t>Testing Support Tasks (Issue Resolution)</t>
-  </si>
-  <si>
-    <t>Analysis &amp; Finalization of Tests</t>
-  </si>
-  <si>
-    <t>5. Deployment to Production</t>
-  </si>
-  <si>
-    <t>5_2 - Configure_Projects_[PROD]</t>
-  </si>
-  <si>
-    <t>Check accounting supplier/customer  party</t>
-  </si>
-  <si>
-    <t>Check  company name validation</t>
-  </si>
-  <si>
-    <t>Check Vat Id validation</t>
-  </si>
-  <si>
-    <t>Check  duplicate source data point</t>
-  </si>
-  <si>
-    <t>(Optional) Check  translation data points if required</t>
-  </si>
-  <si>
-    <t>5_3 - Smoke_test</t>
-  </si>
-  <si>
-    <t>Contact IM to enable newly created [PROD] outbound projects for duplicate check pipeline (Connect projects to IMP pipeline)</t>
-  </si>
-  <si>
-    <t>Contact IM to add outbound projects to XML UBL 2.1 endpoint [PROD]</t>
-  </si>
-  <si>
-    <t>5_4 - Cutover_and_Go_Live</t>
-  </si>
-  <si>
-    <t>Compare project set-up with [TEST] project</t>
-  </si>
-  <si>
-    <t>6_1 - Hypercare_Issues</t>
-  </si>
-  <si>
-    <t>Create and share cutover Plan</t>
-  </si>
-  <si>
     <t>Example File : https://wilhelmsen.sharepoint.com/:x:/r/sites/Wilhelmsen-HypatosDigitalization/Shared%20Documents/General/3.%20-%20Go%20Live/20240321%20WILH%20Cut-Over%20Plan.xlsx?d=we02eb91a059b4632ace3cf0acc7f696a&amp;csf=1&amp;web=1&amp;e=RxxUQ7</t>
   </si>
   <si>
-    <t>Inform customer for Production Readiness &amp;  initiate Production deployment</t>
-  </si>
-  <si>
-    <t>6. Hypercare Phase</t>
-  </si>
-  <si>
-    <t>6_2 - Handover_to_Hypatos_Customer_Care</t>
-  </si>
-  <si>
-    <t>Create and share Hypercare Issue Log</t>
-  </si>
-  <si>
     <t>Example File: https://wilhelmsen.sharepoint.com/:x:/r/sites/Wilhelmsen-HypatosDigitalization/Shared%20Documents/Hypercare%20after%20v1.0%20release/Hypercare%20Issue%20Log.xlsx?d=wfe2e122f9ba146bdaef47f39241aef7e&amp;csf=1&amp;web=1&amp;e=Q4aEIk</t>
   </si>
   <si>
-    <t>Hypercare issue resolutions</t>
-  </si>
-  <si>
-    <t>7_1 - Update_initial_design_sign-off_if_needed,7_2 - Syncronize_Wilhelmsen_Sharepoint_with_Hypatos_Sharepoint</t>
-  </si>
-  <si>
-    <t>Update CC Handover Page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7. Documentation Update </t>
-  </si>
-  <si>
-    <t>7_1 - Update_initial_design_sign-off_if_needed</t>
-  </si>
-  <si>
-    <t>7_2 - Syncronize_Wilhelmsen_Sharepoint_with_Hypatos_Sharepoint</t>
+    <t>Roll-outWilhelmsen</t>
+  </si>
+  <si>
+    <t>0.ProjectManagement</t>
+  </si>
+  <si>
+    <t>0_1-Update_all_related_dates_in_this_project</t>
+  </si>
+  <si>
+    <t>0_2-Update_roll-out_plan</t>
+  </si>
+  <si>
+    <t>0_3-Internal_meetings</t>
+  </si>
+  <si>
+    <t>1.ProcessDiscovery</t>
+  </si>
+  <si>
+    <t>1_1-Data_Acquisition</t>
+  </si>
+  <si>
+    <t>1_2-Requirement_Gathering</t>
+  </si>
+  <si>
+    <t>Training&amp;PostingDataRequest</t>
+  </si>
+  <si>
+    <t>PostingDataAnalysis</t>
+  </si>
+  <si>
+    <t>TrainingDataAssessment</t>
+  </si>
+  <si>
+    <t>Requestadditionaldocumentsifrequired</t>
+  </si>
+  <si>
+    <t>TrainingData/DocumentSetPreparation</t>
+  </si>
+  <si>
+    <t>Matchtrainingdocumentswithpostingdata</t>
+  </si>
+  <si>
+    <t>2_1-Capturing_Model_Training,2_2-Enrichment_Model_Training</t>
+  </si>
+  <si>
+    <t>ProvideDigitalizationDetailsformtoLocalFinanceTeamandaskexamplesforEdgecases</t>
+  </si>
+  <si>
+    <t>ProvideAssessmentGatheringandTrainingDataFolders</t>
+  </si>
+  <si>
+    <t>[ML]DemoProjectCreationforRequirementsGatheringMeeting</t>
+  </si>
+  <si>
+    <t>RequirementGatheringMeeting</t>
+  </si>
+  <si>
+    <t>RequestexamplesforEdgecases</t>
+  </si>
+  <si>
+    <t>Completefullset-upoftrainingdataforallofthetopsupplierswithEdgecasessharedduringrequirementssession</t>
+  </si>
+  <si>
+    <t>UpdateWHLRequirementList</t>
+  </si>
+  <si>
+    <t>RequirementGatheringFinalization</t>
+  </si>
+  <si>
+    <t>2.ModelTraining</t>
+  </si>
+  <si>
+    <t>2_1-Capturing_Model_Training</t>
+  </si>
+  <si>
+    <t>2_3-Model_Fine_Tuning</t>
+  </si>
+  <si>
+    <t>Createbaseline(groundtruth)projecttoannotate[ML]</t>
+  </si>
+  <si>
+    <t>Uploaddocumentsselectedforannotationtogroundtruthproject(TopsuppliersandEdgecases)</t>
+  </si>
+  <si>
+    <t>Createataskforannotation(adddetailsperrequirements)</t>
+  </si>
+  <si>
+    <t>Validateannotationresultswithpostingdata</t>
+  </si>
+  <si>
+    <t>Improveannotationqualitybasedonvalidationwithpostingdata</t>
+  </si>
+  <si>
+    <t>CreateTrainingProject[ML]</t>
+  </si>
+  <si>
+    <t>UploadselectedtrainingdocumentsfrombaselineprojecttoTrainingProject[ML]</t>
+  </si>
+  <si>
+    <t>CreateQAProject[ML]</t>
+  </si>
+  <si>
+    <t>ConfigureQAprojectwithCompositeEnrichmentIndex</t>
+  </si>
+  <si>
+    <t>CreateLLMPromptingService[ML]</t>
+  </si>
+  <si>
+    <t>Uploadbaseline(groundtruth)documentstoQAProject[ML]</t>
+  </si>
+  <si>
+    <t>CreateErrorAnalysisDashboard</t>
+  </si>
+  <si>
+    <t>AnalyzeQAresultsandaccuracy</t>
+  </si>
+  <si>
+    <t>2_2-Enrichment_Model_Training</t>
+  </si>
+  <si>
+    <t>CreateIMPtrainingproject[TEST]</t>
+  </si>
+  <si>
+    <t>ContactwithIMtoenableIMPpipeline</t>
+  </si>
+  <si>
+    <t>UploaddocumentstoIMPtrainingproject</t>
+  </si>
+  <si>
+    <t>TrainsuppliersusingdocumentsuploadedtoIMPproject</t>
+  </si>
+  <si>
+    <t>3_1-Create_Projects_[TEST]</t>
+  </si>
+  <si>
+    <t>Improve/OptimizeLLMPromptingServicepromptwithErrorAnalysisresults</t>
+  </si>
+  <si>
+    <t>AddadditionalsupplierstoIMPprojectifrequired</t>
+  </si>
+  <si>
+    <t>3.StudioConfiguration</t>
+  </si>
+  <si>
+    <t>3_2-Configure_Projects_[TEST]</t>
+  </si>
+  <si>
+    <t>Configureprojectschemawithagreeduponrequirementslistspoints</t>
+  </si>
+  <si>
+    <t>Add/Changeaccountingsupplier/customerparty</t>
+  </si>
+  <si>
+    <t>Add/Changecompanynamevalidation</t>
+  </si>
+  <si>
+    <t>Add/checkvatidvalidation</t>
+  </si>
+  <si>
+    <t>Check/changeduplicatesourcedatapoint</t>
+  </si>
+  <si>
+    <t>(Optional)Addtranslationdatapointsifrequired</t>
+  </si>
+  <si>
+    <t>4_1-Testing_Set-up</t>
+  </si>
+  <si>
+    <t>CreateaCOEtickettoconfigureReroutingrules</t>
+  </si>
+  <si>
+    <t>ContactIMforcompositeenrichmentset-upconfiguration</t>
+  </si>
+  <si>
+    <t>ContactIMtocreateandconfigureLLMpromptingservice</t>
+  </si>
+  <si>
+    <t>ContactIMtoenablenewlycreated[TEST]outboundprojectsforduplicatecheckpipeline(ConnectprojectstoIMPpipeline)</t>
+  </si>
+  <si>
+    <t>ContactIMtoaddoutboundprojectstoXMLUBL2.1endpoint[TEST]</t>
+  </si>
+  <si>
+    <t>ContactIMtoenabletranslationforoutboundprojects</t>
+  </si>
+  <si>
+    <t>4.Testing</t>
+  </si>
+  <si>
+    <t>4_2-Functional_Testing_by_HY</t>
+  </si>
+  <si>
+    <t>CopyandupdateTestWorkbookfornewphaseifneeded</t>
+  </si>
+  <si>
+    <t>4_3-Testing_by_Wilhelmsen</t>
+  </si>
+  <si>
+    <t>Compareprojectset-upwithrequirementslistforspecificcountry</t>
+  </si>
+  <si>
+    <t>UploaddocumentstoGatewayprojectandtestrouting</t>
+  </si>
+  <si>
+    <t>Testadvancedduplicatetesting</t>
+  </si>
+  <si>
+    <t>Testifenrichmentisworkingproperlywithcompanycodefilter</t>
+  </si>
+  <si>
+    <t>TestifXMLendpointifavailableforoutboundprojects(Postman)</t>
+  </si>
+  <si>
+    <t>[Optional]Testtranslationfeature</t>
+  </si>
+  <si>
+    <t>5_1-Create_Projects_[PROD]</t>
+  </si>
+  <si>
+    <t>AddprojectstoRequirementsList</t>
+  </si>
+  <si>
+    <t>ShareTestWorkbook</t>
+  </si>
+  <si>
+    <t>Wilhelmsentoconfigureintegration&amp;performSystemIntegrationTesting(SIT)</t>
+  </si>
+  <si>
+    <t>WilhelmsentoperformFunctionalTesting</t>
+  </si>
+  <si>
+    <t>WilhelmsentoperformUserAcceptanceTesting(UAT)</t>
+  </si>
+  <si>
+    <t>TestingSupportTasks(IssueResolution)</t>
+  </si>
+  <si>
+    <t>Analysis&amp;FinalizationofTests</t>
+  </si>
+  <si>
+    <t>5.DeploymenttoProduction</t>
+  </si>
+  <si>
+    <t>5_2-Configure_Projects_[PROD]</t>
+  </si>
+  <si>
+    <t>Checkaccountingsupplier/customerparty</t>
+  </si>
+  <si>
+    <t>Checkcompanynamevalidation</t>
+  </si>
+  <si>
+    <t>CheckVatIdvalidation</t>
+  </si>
+  <si>
+    <t>Checkduplicatesourcedatapoint</t>
+  </si>
+  <si>
+    <t>(Optional)Checktranslationdatapointsifrequired</t>
+  </si>
+  <si>
+    <t>5_3-Smoke_test</t>
+  </si>
+  <si>
+    <t>ContactIMtoenablenewlycreated[PROD]outboundprojectsforduplicatecheckpipeline(ConnectprojectstoIMPpipeline)</t>
+  </si>
+  <si>
+    <t>ContactIMtoaddoutboundprojectstoXMLUBL2.1endpoint[PROD]</t>
+  </si>
+  <si>
+    <t>5_4-Cutover_and_Go_Live</t>
+  </si>
+  <si>
+    <t>Compareprojectset-upwith[TEST]project</t>
+  </si>
+  <si>
+    <t>6_1-Hypercare_Issues</t>
+  </si>
+  <si>
+    <t>CreateandsharecutoverPlan</t>
+  </si>
+  <si>
+    <t>InformcustomerforProductionReadiness&amp;initiateProductiondeployment</t>
+  </si>
+  <si>
+    <t>6.HypercarePhase</t>
+  </si>
+  <si>
+    <t>6_2-Handover_to_Hypatos_Customer_Care</t>
+  </si>
+  <si>
+    <t>CreateandshareHypercareIssueLog</t>
+  </si>
+  <si>
+    <t>Hypercareissueresolutions</t>
+  </si>
+  <si>
+    <t>7_1-Update_initial_design_sign-off_if_needed,7_2-Syncronize_Wilhelmsen_Sharepoint_with_Hypatos_Sharepoint</t>
+  </si>
+  <si>
+    <t>UpdateCCHandoverPage</t>
+  </si>
+  <si>
+    <t>7.DocumentationUpdate</t>
+  </si>
+  <si>
+    <t>7_1-Update_initial_design_sign-off_if_needed</t>
+  </si>
+  <si>
+    <t>7_2-Syncronize_Wilhelmsen_Sharepoint_with_Hypatos_Sharepoint</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1637,20 +1638,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B2479B-C25A-5C46-8BD3-603EE30C2BE8}">
   <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="97.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="97.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="38.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.95">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1673,12 +1676,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.95">
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
@@ -1686,30 +1689,30 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="15.95">
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" ht="15.95">
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -1718,1700 +1721,1700 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.95">
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G5" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.95">
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G6" s="9">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.95">
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7" ht="15.95">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.95">
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" ht="15.95">
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" ht="15.95">
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" ht="15.95">
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="5" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7" ht="15.95">
+    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="5" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:7" ht="15.95">
+    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="5" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7" ht="15.95">
+    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="47.1" customHeight="1">
+    <row r="16" spans="1:7" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="1:7" ht="224" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" spans="1:7" ht="224.1">
-      <c r="A17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>36</v>
-      </c>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" ht="15.95">
+    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="1:7" ht="15.95">
+    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
     </row>
-    <row r="20" spans="1:7" ht="15.95">
+    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="1:7" ht="15.95">
+    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" spans="1:7" ht="15.95">
+    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="9"/>
       <c r="F22" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="G22" s="9"/>
     </row>
-    <row r="23" spans="1:7" ht="15.95">
+    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
     </row>
-    <row r="24" spans="1:7" ht="15.95">
+    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="1:7" ht="15.95">
+    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.95">
+    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="1:7" ht="15.95">
+    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="1:7" ht="15.95">
+    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:7" ht="15.95">
+    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:7" ht="15.95">
+    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="1:7" ht="15.95">
+    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:7" ht="15.95">
+    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
     </row>
-    <row r="33" spans="1:7" ht="15.95">
+    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
       <c r="F33" s="9" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="G33" s="9"/>
     </row>
-    <row r="34" spans="1:7" ht="15.95">
+    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="1:7" ht="15.95">
+    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
     </row>
-    <row r="36" spans="1:7" ht="15.95">
+    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
     </row>
-    <row r="37" spans="1:7" ht="15.95">
+    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
     </row>
-    <row r="38" spans="1:7" ht="15.95">
+    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
     </row>
-    <row r="39" spans="1:7" ht="15.95">
+    <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.95">
+    <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
     </row>
-    <row r="41" spans="1:7" ht="15.95">
+    <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
     </row>
-    <row r="42" spans="1:7" ht="15.95">
+    <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
     </row>
-    <row r="43" spans="1:7" ht="15.95">
+    <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="8"/>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
     </row>
-    <row r="44" spans="1:7" ht="15.95">
+    <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15.95">
+    <row r="45" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
     </row>
-    <row r="46" spans="1:7" ht="15.95">
+    <row r="46" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="8"/>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
     </row>
-    <row r="47" spans="1:7" ht="15.95">
+    <row r="47" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
     </row>
-    <row r="48" spans="1:7" ht="15.95">
+    <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F48" s="9"/>
       <c r="G48" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="15.95">
+    <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
     </row>
-    <row r="50" spans="1:7" ht="15.95">
+    <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
     </row>
-    <row r="51" spans="1:7" ht="15.95">
+    <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
     </row>
-    <row r="52" spans="1:7" ht="15.95">
+    <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
     </row>
-    <row r="53" spans="1:7" ht="15.95">
+    <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
     </row>
-    <row r="54" spans="1:7" ht="15.95">
+    <row r="54" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
     </row>
-    <row r="55" spans="1:7" ht="15.95">
+    <row r="55" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F55" s="9"/>
       <c r="G55" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15.95">
+    <row r="56" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
       <c r="F56" s="9" t="s">
-        <v>82</v>
+        <v>25</v>
       </c>
       <c r="G56" s="9"/>
     </row>
-    <row r="57" spans="1:7" ht="15.95">
+    <row r="57" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
     </row>
-    <row r="58" spans="1:7" ht="15.95">
+    <row r="58" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
     </row>
-    <row r="59" spans="1:7" ht="15.95">
+    <row r="59" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
     </row>
-    <row r="60" spans="1:7" ht="15.95">
+    <row r="60" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
     </row>
-    <row r="61" spans="1:7" ht="15.95">
+    <row r="61" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
     </row>
-    <row r="62" spans="1:7" ht="15.95">
+    <row r="62" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
     </row>
-    <row r="63" spans="1:7" ht="15.95">
+    <row r="63" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F63" s="9"/>
       <c r="G63" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="15.95">
+    <row r="64" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D64" s="9"/>
       <c r="E64" s="9"/>
       <c r="F64" s="9" t="s">
-        <v>91</v>
+        <v>26</v>
       </c>
       <c r="G64" s="9"/>
     </row>
-    <row r="65" spans="1:7" ht="15.95">
+    <row r="65" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F65" s="9"/>
       <c r="G65" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15.95">
+    <row r="66" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
       <c r="F66" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="G66" s="9"/>
     </row>
-    <row r="67" spans="1:7" ht="15.95">
+    <row r="67" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D67" s="9"/>
       <c r="E67" s="9"/>
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
     </row>
-    <row r="68" spans="1:7" ht="15.95">
+    <row r="68" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
     </row>
-    <row r="69" spans="1:7" ht="15.95">
+    <row r="69" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
     </row>
-    <row r="70" spans="1:7" ht="15.95">
+    <row r="70" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
     </row>
-    <row r="71" spans="1:7" ht="15.95">
+    <row r="71" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
     </row>
-    <row r="72" spans="1:7" ht="15.95">
+    <row r="72" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="D72" s="9" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F72" s="9"/>
       <c r="G72" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15.95">
+    <row r="73" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
     </row>
-    <row r="74" spans="1:7" ht="15.95">
+    <row r="74" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="7"/>
       <c r="F74" s="9" t="s">
-        <v>91</v>
+        <v>26</v>
       </c>
       <c r="G74" s="9"/>
     </row>
-    <row r="75" spans="1:7" ht="15.95">
+    <row r="75" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D75" s="9"/>
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
     </row>
-    <row r="76" spans="1:7" ht="15.95">
+    <row r="76" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D76" s="7"/>
       <c r="E76" s="5"/>
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
     </row>
-    <row r="77" spans="1:7" ht="15.95">
+    <row r="77" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D77" s="9"/>
       <c r="E77" s="9"/>
       <c r="F77" s="9"/>
       <c r="G77" s="9"/>
     </row>
-    <row r="78" spans="1:7" ht="15.95">
+    <row r="78" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D78" s="9"/>
       <c r="E78" s="9"/>
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
     </row>
-    <row r="79" spans="1:7" ht="15.95">
+    <row r="79" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D79" s="9"/>
       <c r="E79" s="9"/>
       <c r="F79" s="9"/>
       <c r="G79" s="9"/>
     </row>
-    <row r="80" spans="1:7" ht="15.95">
+    <row r="80" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
     </row>
-    <row r="81" spans="1:7" ht="15.95">
+    <row r="81" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F81" s="9"/>
       <c r="G81" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15.95">
+    <row r="82" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D82" s="5"/>
       <c r="E82" s="5"/>
       <c r="F82" s="9"/>
       <c r="G82" s="9"/>
     </row>
-    <row r="83" spans="1:7" ht="15.95">
+    <row r="83" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D83" s="9"/>
       <c r="E83" s="9"/>
       <c r="F83" s="9"/>
       <c r="G83" s="9"/>
     </row>
-    <row r="84" spans="1:7" ht="15.95">
+    <row r="84" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
       <c r="F84" s="9"/>
       <c r="G84" s="9"/>
     </row>
-    <row r="85" spans="1:7" ht="15.95">
+    <row r="85" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
       <c r="F85" s="9"/>
       <c r="G85" s="9"/>
     </row>
-    <row r="86" spans="1:7" ht="15.95">
+    <row r="86" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D86" s="9"/>
       <c r="E86" s="9"/>
       <c r="F86" s="9"/>
       <c r="G86" s="9"/>
     </row>
-    <row r="87" spans="1:7" ht="15.95">
+    <row r="87" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D87" s="9"/>
       <c r="E87" s="9"/>
       <c r="F87" s="9"/>
       <c r="G87" s="9"/>
     </row>
-    <row r="88" spans="1:7" ht="15.95">
+    <row r="88" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F88" s="9"/>
       <c r="G88" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15.95">
+    <row r="89" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D89" s="9"/>
       <c r="E89" s="9"/>
       <c r="F89" s="9" t="s">
-        <v>82</v>
+        <v>25</v>
       </c>
       <c r="G89" s="9"/>
     </row>
-    <row r="90" spans="1:7" ht="15.95">
+    <row r="90" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D90" s="9"/>
       <c r="E90" s="9"/>
       <c r="F90" s="9"/>
       <c r="G90" s="9"/>
     </row>
-    <row r="91" spans="1:7" ht="15.95">
+    <row r="91" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
       <c r="F91" s="9"/>
       <c r="G91" s="9"/>
     </row>
-    <row r="92" spans="1:7" ht="15.95">
+    <row r="92" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
       <c r="F92" s="9"/>
       <c r="G92" s="9"/>
     </row>
-    <row r="93" spans="1:7" ht="15.95">
+    <row r="93" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D93" s="9"/>
       <c r="E93" s="9"/>
       <c r="F93" s="9"/>
       <c r="G93" s="9"/>
     </row>
-    <row r="94" spans="1:7" ht="15.95">
+    <row r="94" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D94" s="9"/>
       <c r="E94" s="9"/>
       <c r="F94" s="9"/>
       <c r="G94" s="9"/>
     </row>
-    <row r="95" spans="1:7" ht="15.95">
+    <row r="95" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F95" s="9"/>
       <c r="G95" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15.95">
+    <row r="96" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D96" s="5"/>
       <c r="E96" s="5"/>
       <c r="F96" s="9"/>
       <c r="G96" s="9"/>
     </row>
-    <row r="97" spans="1:7" ht="15.95">
+    <row r="97" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D97" s="9"/>
       <c r="E97" s="9"/>
       <c r="F97" s="9"/>
       <c r="G97" s="9"/>
     </row>
-    <row r="98" spans="1:7" ht="15.95">
+    <row r="98" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D98" s="9"/>
       <c r="E98" s="9"/>
       <c r="F98" s="9"/>
       <c r="G98" s="9"/>
     </row>
-    <row r="99" spans="1:7" ht="15.95">
+    <row r="99" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D99" s="5"/>
       <c r="E99" s="5"/>
       <c r="F99" s="9"/>
       <c r="G99" s="9"/>
     </row>
-    <row r="100" spans="1:7" ht="15.95">
+    <row r="100" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D100" s="5"/>
       <c r="E100" s="5"/>
       <c r="F100" s="9"/>
       <c r="G100" s="9"/>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="15.95">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G102" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F103" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F104" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="104" spans="1:7">
-      <c r="A104" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F104" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7">
-      <c r="A105" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7">
-      <c r="A106" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="15.95">
-      <c r="A107" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="B107" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D107" s="9" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E107" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G107" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="15.95">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C110" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B110" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="D110" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E110" s="9" t="s">
         <v>129</v>
@@ -3420,34 +3423,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>130</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>131</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" ht="15.95">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>131</v>
@@ -3458,12 +3461,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="15.95">
+    <row r="114" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>131</v>
@@ -3476,181 +3479,532 @@
   </sheetData>
   <autoFilter ref="A1:G114" xr:uid="{C0B2479B-C25A-5C46-8BD3-603EE30C2BE8}"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="76" priority="104"/>
-    <cfRule type="duplicateValues" dxfId="75" priority="105"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
+    <cfRule type="duplicateValues" dxfId="76" priority="105"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="104"/>
     <cfRule type="duplicateValues" dxfId="74" priority="39"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="duplicateValues" dxfId="73" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="duplicateValues" dxfId="71" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3">
+    <cfRule type="duplicateValues" dxfId="69" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="duplicateValues" dxfId="67" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="duplicateValues" dxfId="65" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="duplicateValues" dxfId="63" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
+    <cfRule type="duplicateValues" dxfId="61" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C80">
+    <cfRule type="duplicateValues" dxfId="59" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C106">
+    <cfRule type="duplicateValues" dxfId="57" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C112">
+    <cfRule type="duplicateValues" dxfId="55" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="duplicateValues" dxfId="73" priority="112"/>
-    <cfRule type="duplicateValues" dxfId="72" priority="113"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="112"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="113"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="duplicateValues" dxfId="71" priority="114"/>
-    <cfRule type="duplicateValues" dxfId="70" priority="115"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="114"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="115"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="duplicateValues" dxfId="69" priority="30"/>
-    <cfRule type="duplicateValues" dxfId="68" priority="31"/>
-    <cfRule type="duplicateValues" dxfId="67" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="duplicateValues" dxfId="66" priority="118"/>
-    <cfRule type="duplicateValues" dxfId="65" priority="119"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="118"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="119"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="duplicateValues" dxfId="64" priority="36"/>
-    <cfRule type="duplicateValues" dxfId="63" priority="37"/>
-    <cfRule type="duplicateValues" dxfId="62" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="duplicateValues" dxfId="61" priority="102"/>
-    <cfRule type="duplicateValues" dxfId="60" priority="103"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="103"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="102"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="duplicateValues" dxfId="59" priority="122"/>
-    <cfRule type="duplicateValues" dxfId="58" priority="123"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="123"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="122"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="duplicateValues" dxfId="57" priority="98"/>
-    <cfRule type="duplicateValues" dxfId="56" priority="99"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="99"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="98"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43">
-    <cfRule type="duplicateValues" dxfId="55" priority="46"/>
-    <cfRule type="duplicateValues" dxfId="54" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="duplicateValues" dxfId="53" priority="124"/>
-    <cfRule type="duplicateValues" dxfId="52" priority="125"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="125"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="124"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62">
-    <cfRule type="duplicateValues" dxfId="51" priority="100"/>
-    <cfRule type="duplicateValues" dxfId="50" priority="101"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="100"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="101"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D74">
-    <cfRule type="duplicateValues" dxfId="49" priority="92"/>
-    <cfRule type="duplicateValues" dxfId="48" priority="93"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="92"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="93"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="duplicateValues" dxfId="47" priority="54"/>
-    <cfRule type="duplicateValues" dxfId="46" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="duplicateValues" dxfId="45" priority="116"/>
-    <cfRule type="duplicateValues" dxfId="44" priority="117"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="117"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="116"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="duplicateValues" dxfId="43" priority="24"/>
-    <cfRule type="duplicateValues" dxfId="42" priority="25"/>
-    <cfRule type="duplicateValues" dxfId="41" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="duplicateValues" dxfId="40" priority="50"/>
-    <cfRule type="duplicateValues" dxfId="39" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="duplicateValues" dxfId="38" priority="33"/>
-    <cfRule type="duplicateValues" dxfId="37" priority="34"/>
-    <cfRule type="duplicateValues" dxfId="36" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="duplicateValues" dxfId="35" priority="96"/>
-    <cfRule type="duplicateValues" dxfId="34" priority="97"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="96"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="duplicateValues" dxfId="33" priority="48"/>
-    <cfRule type="duplicateValues" dxfId="32" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46">
-    <cfRule type="duplicateValues" dxfId="31" priority="126"/>
-    <cfRule type="duplicateValues" dxfId="30" priority="127"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="126"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="127"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62">
-    <cfRule type="duplicateValues" dxfId="29" priority="88"/>
-    <cfRule type="duplicateValues" dxfId="28" priority="89"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="89"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="88"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74">
-    <cfRule type="duplicateValues" dxfId="27" priority="90"/>
-    <cfRule type="duplicateValues" dxfId="26" priority="91"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="91"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="90"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E76">
-    <cfRule type="duplicateValues" dxfId="25" priority="82"/>
-    <cfRule type="duplicateValues" dxfId="24" priority="83"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="83"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="82"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85">
-    <cfRule type="duplicateValues" dxfId="23" priority="78"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="79"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="79"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="78"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E91 E99">
-    <cfRule type="duplicateValues" dxfId="21" priority="44"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="45"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="19" priority="19"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="20"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="duplicateValues" dxfId="17" priority="17"/>
-    <cfRule type="duplicateValues" dxfId="16" priority="18"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3">
-    <cfRule type="duplicateValues" dxfId="15" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="14" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
-    <cfRule type="duplicateValues" dxfId="13" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="14"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C80">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C106">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C112">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="44"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2d57a97e-bf0b-4cec-a587-841817f75a75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d57067be-9d14-4795-a8ab-0027d10e2a03" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBEE0DB8-683A-5E4D-9A10-1C52794522C7}">
+  <dimension ref="A1:A108"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A108"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.6640625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+    </row>
+    <row r="3" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="9"/>
+    </row>
+    <row r="4" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="9"/>
+    </row>
+    <row r="5" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="9"/>
+    </row>
+    <row r="8" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="6"/>
+    </row>
+    <row r="9" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="9"/>
+    </row>
+    <row r="16" spans="1:1" ht="187" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="224" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="9"/>
+    </row>
+    <row r="20" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="9"/>
+    </row>
+    <row r="21" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="9"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="9"/>
+    </row>
+    <row r="24" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="9"/>
+    </row>
+    <row r="25" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="9"/>
+    </row>
+    <row r="26" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="9"/>
+    </row>
+    <row r="28" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="9"/>
+    </row>
+    <row r="29" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="9"/>
+    </row>
+    <row r="30" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="9"/>
+    </row>
+    <row r="31" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="9"/>
+    </row>
+    <row r="33" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="9"/>
+    </row>
+    <row r="35" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="9"/>
+    </row>
+    <row r="36" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="9"/>
+    </row>
+    <row r="37" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="9"/>
+    </row>
+    <row r="38" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="9"/>
+    </row>
+    <row r="39" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="9"/>
+    </row>
+    <row r="40" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="9"/>
+    </row>
+    <row r="41" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="9"/>
+    </row>
+    <row r="42" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="9"/>
+    </row>
+    <row r="43" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="9"/>
+    </row>
+    <row r="44" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="9"/>
+    </row>
+    <row r="45" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="9"/>
+    </row>
+    <row r="46" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="9"/>
+    </row>
+    <row r="47" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="9"/>
+    </row>
+    <row r="48" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="9"/>
+    </row>
+    <row r="49" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="9"/>
+    </row>
+    <row r="50" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="9"/>
+    </row>
+    <row r="51" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="9"/>
+    </row>
+    <row r="52" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="9"/>
+    </row>
+    <row r="53" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="9"/>
+    </row>
+    <row r="54" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="9"/>
+    </row>
+    <row r="55" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="9"/>
+    </row>
+    <row r="56" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="9"/>
+    </row>
+    <row r="58" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="9"/>
+    </row>
+    <row r="59" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="9"/>
+    </row>
+    <row r="60" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="9"/>
+    </row>
+    <row r="61" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="9"/>
+    </row>
+    <row r="62" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="9"/>
+    </row>
+    <row r="63" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="9"/>
+    </row>
+    <row r="64" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" s="9"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="9"/>
+    </row>
+    <row r="68" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" s="9"/>
+    </row>
+    <row r="69" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="9"/>
+    </row>
+    <row r="70" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A70" s="9"/>
+    </row>
+    <row r="71" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A71" s="9"/>
+    </row>
+    <row r="72" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" s="9"/>
+    </row>
+    <row r="73" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A73" s="9"/>
+    </row>
+    <row r="74" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A74" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A75" s="9"/>
+    </row>
+    <row r="76" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A76" s="9"/>
+    </row>
+    <row r="77" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A77" s="9"/>
+    </row>
+    <row r="78" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A78" s="9"/>
+    </row>
+    <row r="79" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A79" s="9"/>
+    </row>
+    <row r="80" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A80" s="9"/>
+    </row>
+    <row r="81" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A81" s="9"/>
+    </row>
+    <row r="82" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A82" s="9"/>
+    </row>
+    <row r="83" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A83" s="9"/>
+    </row>
+    <row r="84" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A84" s="9"/>
+    </row>
+    <row r="85" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A85" s="9"/>
+    </row>
+    <row r="86" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A86" s="9"/>
+    </row>
+    <row r="87" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A87" s="9"/>
+    </row>
+    <row r="88" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A88" s="9"/>
+    </row>
+    <row r="89" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A89" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A90" s="9"/>
+    </row>
+    <row r="91" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A91" s="9"/>
+    </row>
+    <row r="92" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A92" s="9"/>
+    </row>
+    <row r="93" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A93" s="9"/>
+    </row>
+    <row r="94" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" s="9"/>
+    </row>
+    <row r="95" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A95" s="9"/>
+    </row>
+    <row r="96" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A96" s="9"/>
+    </row>
+    <row r="97" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A97" s="9"/>
+    </row>
+    <row r="98" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A98" s="9"/>
+    </row>
+    <row r="99" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A99" s="9"/>
+    </row>
+    <row r="100" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A100" s="9"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100541D480877BA4048A9D91342E163CE04" ma:contentTypeVersion="19" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="28d96b37b54d0536772fb70d3e350a96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2d57a97e-bf0b-4cec-a587-841817f75a75" xmlns:ns3="d57067be-9d14-4795-a8ab-0027d10e2a03" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2f1fc382afb7be30a231b340c6285373" ns2:_="" ns3:_="">
     <xsd:import namespace="2d57a97e-bf0b-4cec-a587-841817f75a75"/>
@@ -3905,14 +4259,60 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2d57a97e-bf0b-4cec-a587-841817f75a75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d57067be-9d14-4795-a8ab-0027d10e2a03" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5EEA4BE-BEF6-40EB-9E91-95E267084DF6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{702467FC-0767-4CD6-B1F3-E30D48499054}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2d57a97e-bf0b-4cec-a587-841817f75a75"/>
+    <ds:schemaRef ds:uri="d57067be-9d14-4795-a8ab-0027d10e2a03"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62374C78-7643-457E-861B-A603D8D81D7C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62374C78-7643-457E-861B-A603D8D81D7C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{702467FC-0767-4CD6-B1F3-E30D48499054}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5EEA4BE-BEF6-40EB-9E91-95E267084DF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2d57a97e-bf0b-4cec-a587-841817f75a75"/>
+    <ds:schemaRef ds:uri="d57067be-9d14-4795-a8ab-0027d10e2a03"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>